<commit_message>
fixed bugs + functionality
</commit_message>
<xml_diff>
--- a/Stock Screener.xlsx
+++ b/Stock Screener.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spenc\VSCode\Stock-Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934D685D-C74D-4D74-9820-39129830FA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4511B488-EB57-4EFC-8A03-2D04ECE50139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>#</t>
   </si>
@@ -64,27 +64,6 @@
   </si>
   <si>
     <t>Rating</t>
-  </si>
-  <si>
-    <t>TD.TO</t>
-  </si>
-  <si>
-    <t>RY.TO</t>
-  </si>
-  <si>
-    <t>QQQ</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>TRP.TO</t>
-  </si>
-  <si>
-    <t>SPXEFR</t>
   </si>
 </sst>
 </file>
@@ -409,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,41 +444,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Set 'Mixed' as default strat
</commit_message>
<xml_diff>
--- a/Stock Screener.xlsx
+++ b/Stock Screener.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spenc\VSCode\Python\Stock-Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F920EE1-8DF0-4257-96D0-7388341EBC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C8FF3E-4387-461A-8F97-BE598438ED76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Select strategy from terminal
</commit_message>
<xml_diff>
--- a/Stock Screener.xlsx
+++ b/Stock Screener.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spenc\VSCode\Python\Stock-Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AABD258-1801-4CA9-9508-EBF726A7F64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96E5CA7-BD44-4B55-A3D1-9C5CDDB24C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>#</t>
   </si>
@@ -56,6 +56,21 @@
   </si>
   <si>
     <t>52W High</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>SMCI</t>
+  </si>
+  <si>
+    <t>SHOP.TO</t>
+  </si>
+  <si>
+    <t>BTC-USD</t>
+  </si>
+  <si>
+    <t>I like cats</t>
   </si>
 </sst>
 </file>
@@ -394,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,7 +466,9 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -466,7 +483,9 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -481,7 +500,9 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -496,7 +517,9 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -508,6 +531,11 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>